<commit_message>
feat: Remove LiveChat widget and add Conversation Quality Check page
Changes:
1. Removed LiveChat widget from index.html
2. Added '对话质检' navigation item in Layout.tsx
3. Created ConversationQualityPage.tsx with draft UI:
   - Input section: text area and file upload (.txt)
   - Result section: displays quality tag (resolved/partially_resolved/unresolved)
   - Confidence score with progress bar
   - Analysis reasoning display
   - Action buttons (clear, re-analyze)
   - Info section explaining the three quality levels
4. Added route for /quality in App.tsx

UI Features:
- Two-column responsive layout
- Animated transitions using Framer Motion
- Color-coded tags (green/yellow/red)
- Confidence score visualization
- File upload support
- Loading states
- Error handling
- Mock analysis for demonstration
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>input</t>
   </si>
@@ -38,7 +38,13 @@
     <t>hi</t>
   </si>
   <si>
-    <t>ai怎么赋能客户系统</t>
+    <t>你是哪个模型厂商提供的</t>
+  </si>
+  <si>
+    <t>只切一刀，如何把四个橘子分给四个小朋友？</t>
+  </si>
+  <si>
+    <t>我拿水兑水，得到的是稀水还是浓水？</t>
   </si>
 </sst>
 </file>
@@ -1191,13 +1197,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.3846153846154" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="10.3846153846154" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1217,6 +1223,16 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>